<commit_message>
update DB_mock, sign_up.html and add 2file
</commit_message>
<xml_diff>
--- a/public/BK_mockup/DB_mock.xlsx
+++ b/public/BK_mockup/DB_mock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\student\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D1BA1E-9995-47C2-962C-0311D80B3D8D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC79FAED-44CF-469D-A0C0-E02E700D3221}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" activeTab="1" xr2:uid="{656A00BE-8496-4AAC-8B53-AB99A01A0A5A}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
   <si>
     <t>入出金テーブル</t>
     <rPh sb="0" eb="3">
@@ -36,10 +36,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>user ID</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>ユーザーテーブル</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -101,6 +97,80 @@
   </si>
   <si>
     <t>regist_id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>カラム名</t>
+    <rPh sb="3" eb="4">
+      <t>メイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>データ型</t>
+    <rPh sb="3" eb="4">
+      <t>ガタ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>INT</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>VARCHAR(255)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DATE</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>備考</t>
+    <rPh sb="0" eb="2">
+      <t>ビコウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>null許可</t>
+    <rPh sb="4" eb="6">
+      <t>キョカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>同一</t>
+    <rPh sb="0" eb="2">
+      <t>ドウイツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>regist_table</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>user_table</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>tag_table</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>VARCHAR(32)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>primary</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>auto_increment</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -143,12 +213,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -165,7 +247,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -173,6 +255,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -489,44 +577,105 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F576665E-E7AD-4326-8358-37DCE6719C0D}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
+    <col min="2" max="2" width="15.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="25.5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="25.5" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A2" s="1" t="s">
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
-        <v>11</v>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>8</v>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B7" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -538,48 +687,98 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39C2AB84-953F-471E-A727-757DD778570F}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="6.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="25.5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="25.5" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" t="s">
-        <v>9</v>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B7" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -591,32 +790,64 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C556F62-CD00-4B77-99CD-C3B4610EABF2}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="18.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="25.5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="25.5" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>